<commit_message>
fix xlsx client, remove models extensions
</commit_message>
<xml_diff>
--- a/PLVisualizerTest/TestDocxClient/docxtest.xlsx
+++ b/PLVisualizerTest/TestDocxClient/docxtest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="42">
   <si>
     <t xml:space="preserve">Учебный период</t>
   </si>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Факультет математико-механический</t>
   </si>
   <si>
-    <t xml:space="preserve">№5665,2022: Математическое обеспечение и администрирование информационных систем</t>
+    <t xml:space="preserve">№5665,2021: Математическое обеспечение и администрирование информационных систем</t>
   </si>
   <si>
     <t xml:space="preserve">002212 Программирование</t>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t xml:space="preserve">Кириленко Яков Александрович</t>
-  </si>
-  <si>
-    <t xml:space="preserve">№5665,2021: Математическое обеспечение и администрирование информационных систем</t>
   </si>
   <si>
     <t xml:space="preserve">002187 Структуры и алгоритмы компьютерной обработки данных</t>
@@ -252,8 +249,8 @@
   </sheetPr>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O16" activeCellId="0" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1222,7 +1219,7 @@
         <v>16</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1251,7 +1248,7 @@
         <v>16</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,10 +1259,10 @@
         <v>10</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>25</v>
@@ -1309,7 +1306,7 @@
         <v>16</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1320,10 +1317,10 @@
         <v>10</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>26</v>

</xml_diff>